<commit_message>
Add missing images in EXCEL file (and update csv accordingly)
</commit_message>
<xml_diff>
--- a/resources/4_mei_encoding/Iberian_square_notation/SQUAREnotation-NClevel.xlsx
+++ b/resources/4_mei_encoding/Iberian_square_notation/SQUAREnotation-NClevel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/OMR_Portuguese_Sources/resources/4_mei_encoding/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marthae.thomae/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B497F2D6-34FC-9841-B151-A2D342D09C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17026047-8493-DF40-860B-C37B2F74BFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="7960" windowWidth="38220" windowHeight="17440" xr2:uid="{C592A449-FCA0-F446-94A9-8EE74258CB16}"/>
+    <workbookView xWindow="7960" yWindow="740" windowWidth="21440" windowHeight="16880" xr2:uid="{C592A449-FCA0-F446-94A9-8EE74258CB16}"/>
   </bookViews>
   <sheets>
     <sheet name="SQUAREnotation-NClevel_2" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="12">
+  <futureMetadata name="XLRICHVALUE" count="22">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -122,8 +122,78 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="12"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="13"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="14"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="15"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="16"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="17"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="18"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="19"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="20"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="21"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="12">
+  <valueMetadata count="22">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -159,13 +229,43 @@
     </bk>
     <bk>
       <rc t="1" v="11"/>
+    </bk>
+    <bk>
+      <rc t="1" v="12"/>
+    </bk>
+    <bk>
+      <rc t="1" v="13"/>
+    </bk>
+    <bk>
+      <rc t="1" v="14"/>
+    </bk>
+    <bk>
+      <rc t="1" v="15"/>
+    </bk>
+    <bk>
+      <rc t="1" v="16"/>
+    </bk>
+    <bk>
+      <rc t="1" v="17"/>
+    </bk>
+    <bk>
+      <rc t="1" v="18"/>
+    </bk>
+    <bk>
+      <rc t="1" v="19"/>
+    </bk>
+    <bk>
+      <rc t="1" v="20"/>
+    </bk>
+    <bk>
+      <rc t="1" v="21"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="113">
   <si>
     <t>imagePath</t>
   </si>
@@ -558,6 +658,9 @@
     &lt;nc type="twolegsdown"/&gt;
     &lt;nc intm="0S" type="twolegsdown"/&gt;
 &lt;/neume&gt;</t>
+  </si>
+  <si>
+    <t>144-145</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1260,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="12">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="22">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -1206,6 +1309,46 @@
     <v>11</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>13</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>14</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>15</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>16</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>17</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>18</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>19</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>20</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>21</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -1232,6 +1375,16 @@
   <rel r:id="rId10"/>
   <rel r:id="rId11"/>
   <rel r:id="rId12"/>
+  <rel r:id="rId13"/>
+  <rel r:id="rId14"/>
+  <rel r:id="rId15"/>
+  <rel r:id="rId16"/>
+  <rel r:id="rId17"/>
+  <rel r:id="rId18"/>
+  <rel r:id="rId19"/>
+  <rel r:id="rId20"/>
+  <rel r:id="rId21"/>
+  <rel r:id="rId22"/>
 </richValueRels>
 </file>
 
@@ -1554,8 +1707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC82D83-23D5-EB47-B9BB-AA65280E3DDF}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2025,12 +2178,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="116" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B14" t="s">
-        <v>17</v>
+      <c r="B14" t="e" vm="13">
+        <v>#VALUE!</v>
       </c>
       <c r="C14" t="s">
         <v>77</v>
@@ -2039,7 +2192,7 @@
         <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="F14" t="s">
         <v>78</v>
@@ -2057,15 +2210,15 @@
         <v>17</v>
       </c>
       <c r="K14" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
-        <v>17</v>
+      <c r="B15" t="e" vm="14">
+        <v>#VALUE!</v>
       </c>
       <c r="C15" t="s">
         <v>80</v>
@@ -2074,7 +2227,7 @@
         <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="F15" t="s">
         <v>81</v>
@@ -2092,15 +2245,15 @@
         <v>17</v>
       </c>
       <c r="K15" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
-        <v>17</v>
+      <c r="B16" t="e" vm="15">
+        <v>#VALUE!</v>
       </c>
       <c r="C16" t="s">
         <v>83</v>
@@ -2109,7 +2262,7 @@
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="F16" t="s">
         <v>84</v>
@@ -2127,15 +2280,15 @@
         <v>17</v>
       </c>
       <c r="K16" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
-        <v>17</v>
+      <c r="B17" t="e" vm="16">
+        <v>#VALUE!</v>
       </c>
       <c r="C17" t="s">
         <v>86</v>
@@ -2144,7 +2297,7 @@
         <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="F17" t="s">
         <v>87</v>
@@ -2162,15 +2315,15 @@
         <v>17</v>
       </c>
       <c r="K17" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="94" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>17</v>
+      <c r="B18" t="e" vm="17">
+        <v>#VALUE!</v>
       </c>
       <c r="C18" t="s">
         <v>89</v>
@@ -2179,7 +2332,7 @@
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="F18" t="s">
         <v>90</v>
@@ -2197,15 +2350,15 @@
         <v>17</v>
       </c>
       <c r="K18" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>17</v>
+      <c r="B19" t="e" vm="18">
+        <v>#VALUE!</v>
       </c>
       <c r="C19" t="s">
         <v>92</v>
@@ -2214,7 +2367,7 @@
         <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="F19" t="s">
         <v>93</v>
@@ -2232,15 +2385,15 @@
         <v>17</v>
       </c>
       <c r="K19" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" t="s">
-        <v>17</v>
+      <c r="B20" t="e" vm="19">
+        <v>#VALUE!</v>
       </c>
       <c r="C20" t="s">
         <v>96</v>
@@ -2249,7 +2402,7 @@
         <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="F20" t="s">
         <v>97</v>
@@ -2267,15 +2420,15 @@
         <v>17</v>
       </c>
       <c r="K20" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B21" t="s">
-        <v>17</v>
+      <c r="B21" t="e" vm="20">
+        <v>#VALUE!</v>
       </c>
       <c r="C21" t="s">
         <v>99</v>
@@ -2284,7 +2437,7 @@
         <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="F21" t="s">
         <v>100</v>
@@ -2302,15 +2455,15 @@
         <v>17</v>
       </c>
       <c r="K21" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="B22" t="s">
-        <v>17</v>
+      <c r="B22" t="e" vm="21">
+        <v>#VALUE!</v>
       </c>
       <c r="C22" t="s">
         <v>101</v>
@@ -2319,7 +2472,7 @@
         <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="F22" t="s">
         <v>102</v>
@@ -2337,15 +2490,15 @@
         <v>17</v>
       </c>
       <c r="K22" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="B23" t="s">
-        <v>17</v>
+      <c r="B23" t="e" vm="22">
+        <v>#VALUE!</v>
       </c>
       <c r="C23" t="s">
         <v>104</v>
@@ -2354,7 +2507,7 @@
         <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="F23" t="s">
         <v>105</v>
@@ -2372,7 +2525,7 @@
         <v>17</v>
       </c>
       <c r="K23" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="85" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update order of neumes in table (square)
</commit_message>
<xml_diff>
--- a/resources/4_mei_encoding/Iberian_square_notation/SQUAREnotation-NClevel.xlsx
+++ b/resources/4_mei_encoding/Iberian_square_notation/SQUAREnotation-NClevel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marthae.thomae/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marthae.thomae/Downloads/OMR_Portuguese_Sources/resources/4_mei_encoding/Iberian_square_notation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17026047-8493-DF40-860B-C37B2F74BFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A78788-7230-1349-A656-91014D357710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7960" yWindow="740" windowWidth="21440" windowHeight="16880" xr2:uid="{C592A449-FCA0-F446-94A9-8EE74258CB16}"/>
+    <workbookView xWindow="7740" yWindow="740" windowWidth="21660" windowHeight="16880" xr2:uid="{C592A449-FCA0-F446-94A9-8EE74258CB16}"/>
   </bookViews>
   <sheets>
     <sheet name="SQUAREnotation-NClevel_2" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="115">
   <si>
     <t>imagePath</t>
   </si>
@@ -661,6 +661,12 @@
   </si>
   <si>
     <t>144-145</t>
+  </si>
+  <si>
+    <t>[no link]</t>
+  </si>
+  <si>
+    <t>[no image]</t>
   </si>
 </sst>
 </file>
@@ -1707,8 +1713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC82D83-23D5-EB47-B9BB-AA65280E3DDF}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1758,30 +1764,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
+    <row r="2" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>113</v>
       </c>
       <c r="B2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
+      <c r="H2" t="s">
+        <v>79</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
@@ -1790,33 +1796,33 @@
         <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>19</v>
+    <row r="3" spans="1:11" ht="77" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>113</v>
       </c>
       <c r="B3" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3">
-        <v>27</v>
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>23</v>
+      <c r="H3" t="s">
+        <v>82</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
@@ -1825,33 +1831,33 @@
         <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>25</v>
+    <row r="4" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>113</v>
       </c>
       <c r="B4" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>29</v>
+      <c r="H4" t="s">
+        <v>85</v>
       </c>
       <c r="I4" t="s">
         <v>17</v>
@@ -1860,33 +1866,33 @@
         <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>30</v>
+    <row r="5" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>113</v>
       </c>
       <c r="B5" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5">
-        <v>355</v>
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>88</v>
       </c>
       <c r="I5" t="s">
         <v>17</v>
@@ -1895,33 +1901,33 @@
         <v>17</v>
       </c>
       <c r="K5" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>35</v>
+    <row r="6" spans="1:11" ht="94" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>113</v>
       </c>
       <c r="B6" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6">
-        <v>348</v>
+        <v>89</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>39</v>
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>91</v>
       </c>
       <c r="I6" t="s">
         <v>17</v>
@@ -1930,33 +1936,33 @@
         <v>17</v>
       </c>
       <c r="K6" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B7" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7">
-        <v>131</v>
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="I7" t="s">
         <v>17</v>
@@ -1965,33 +1971,33 @@
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B8" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D8">
-        <v>348</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="I8" t="s">
         <v>17</v>
@@ -2003,30 +2009,30 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B9" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="I9" t="s">
         <v>17</v>
@@ -2038,30 +2044,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B10" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D10">
         <v>348</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" t="s">
-        <v>94</v>
+        <v>48</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
@@ -2073,30 +2079,30 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B11" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11">
-        <v>91</v>
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I11" t="s">
         <v>17</v>
@@ -2105,33 +2111,33 @@
         <v>17</v>
       </c>
       <c r="K11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>66</v>
+    <row r="12" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>113</v>
       </c>
       <c r="B12" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12">
-        <v>12</v>
+        <v>92</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="F12" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="I12" t="s">
         <v>17</v>
@@ -2140,33 +2146,33 @@
         <v>17</v>
       </c>
       <c r="K12" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>71</v>
+    <row r="13" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>113</v>
       </c>
       <c r="B13" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
+        <v>96</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="F13" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="I13" t="s">
         <v>17</v>
@@ -2178,30 +2184,30 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="116" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>17</v>
+    <row r="14" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B14" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
+        <v>57</v>
+      </c>
+      <c r="D14">
+        <v>348</v>
       </c>
       <c r="E14" t="s">
-        <v>112</v>
+        <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>79</v>
+        <v>59</v>
+      </c>
+      <c r="G14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="I14" t="s">
         <v>17</v>
@@ -2210,18 +2216,18 @@
         <v>17</v>
       </c>
       <c r="K14" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="109" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="B15" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -2230,13 +2236,13 @@
         <v>112</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
-        <v>82</v>
+        <v>100</v>
+      </c>
+      <c r="G15" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="I15" t="s">
         <v>17</v>
@@ -2248,30 +2254,30 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="83" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>17</v>
+    <row r="16" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B16" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
+        <v>31</v>
+      </c>
+      <c r="D16">
+        <v>355</v>
       </c>
       <c r="E16" t="s">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="I16" t="s">
         <v>17</v>
@@ -2280,33 +2286,33 @@
         <v>17</v>
       </c>
       <c r="K16" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>17</v>
+    <row r="17" spans="1:11" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B17" t="e" vm="16">
         <v>#VALUE!</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
+        <v>36</v>
+      </c>
+      <c r="D17">
+        <v>348</v>
       </c>
       <c r="E17" t="s">
-        <v>112</v>
+        <v>37</v>
       </c>
       <c r="F17" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>88</v>
+        <v>2</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="I17" t="s">
         <v>17</v>
@@ -2315,33 +2321,33 @@
         <v>17</v>
       </c>
       <c r="K17" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="94" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
+    <row r="18" spans="1:11" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B18" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
+        <v>41</v>
+      </c>
+      <c r="D18">
+        <v>131</v>
       </c>
       <c r="E18" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="F18" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>91</v>
+        <v>2</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="I18" t="s">
         <v>17</v>
@@ -2350,33 +2356,33 @@
         <v>17</v>
       </c>
       <c r="K18" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>17</v>
+    <row r="19" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="B19" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
+        <v>61</v>
+      </c>
+      <c r="D19">
+        <v>91</v>
       </c>
       <c r="E19" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="F19" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="I19" t="s">
         <v>17</v>
@@ -2385,33 +2391,33 @@
         <v>17</v>
       </c>
       <c r="K19" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>17</v>
+    <row r="20" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="B20" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
+        <v>67</v>
+      </c>
+      <c r="D20">
+        <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="F20" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="I20" t="s">
         <v>17</v>
@@ -2420,33 +2426,33 @@
         <v>17</v>
       </c>
       <c r="K20" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>17</v>
+      <c r="A21" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="B21" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" t="s">
-        <v>17</v>
+        <v>72</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="F21" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="I21" t="s">
         <v>17</v>
@@ -2460,7 +2466,7 @@
     </row>
     <row r="22" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="B22" t="e" vm="21">
         <v>#VALUE!</v>
@@ -2495,7 +2501,7 @@
     </row>
     <row r="23" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="B23" t="e" vm="22">
         <v>#VALUE!</v>
@@ -2530,10 +2536,10 @@
     </row>
     <row r="24" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="C24" t="s">
         <v>107</v>
@@ -2565,18 +2571,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{F3BF08D0-E2E5-7F47-AECB-0E93C29F96E6}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{CBF7E167-8FEF-5B4A-8789-7FD2483C3BC2}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{E656D62C-D5A0-B64A-97AF-FE410AD9D51D}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{E197226A-C9AF-9845-BEF9-F22CFD2DF8AB}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{1B38313D-BE78-BA43-BC12-28BBC38EDEE9}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{7AAB5EA4-19C7-344E-9B13-8104F7F93F9C}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{E2B356D1-FE04-A74B-83B1-7AD174F763CD}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{19C592A9-96EC-D449-8955-168C04FE19F9}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{F98FD0C2-1838-454E-87CA-84211B5E6D50}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{C73AE674-942C-9948-AF90-C512E30D1A38}"/>
-    <hyperlink ref="A12" r:id="rId11" xr:uid="{A9591B94-087A-A748-AD59-ECCA265930F6}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{C49F1946-962B-0849-89CF-B07B6FCF213D}"/>
+    <hyperlink ref="A7" r:id="rId1" xr:uid="{F3BF08D0-E2E5-7F47-AECB-0E93C29F96E6}"/>
+    <hyperlink ref="A8" r:id="rId2" xr:uid="{CBF7E167-8FEF-5B4A-8789-7FD2483C3BC2}"/>
+    <hyperlink ref="A9" r:id="rId3" xr:uid="{E656D62C-D5A0-B64A-97AF-FE410AD9D51D}"/>
+    <hyperlink ref="A16" r:id="rId4" xr:uid="{E197226A-C9AF-9845-BEF9-F22CFD2DF8AB}"/>
+    <hyperlink ref="A17" r:id="rId5" xr:uid="{1B38313D-BE78-BA43-BC12-28BBC38EDEE9}"/>
+    <hyperlink ref="A18" r:id="rId6" xr:uid="{7AAB5EA4-19C7-344E-9B13-8104F7F93F9C}"/>
+    <hyperlink ref="A10" r:id="rId7" xr:uid="{E2B356D1-FE04-A74B-83B1-7AD174F763CD}"/>
+    <hyperlink ref="A11" r:id="rId8" xr:uid="{19C592A9-96EC-D449-8955-168C04FE19F9}"/>
+    <hyperlink ref="A14" r:id="rId9" xr:uid="{F98FD0C2-1838-454E-87CA-84211B5E6D50}"/>
+    <hyperlink ref="A19" r:id="rId10" xr:uid="{C73AE674-942C-9948-AF90-C512E30D1A38}"/>
+    <hyperlink ref="A20" r:id="rId11" xr:uid="{A9591B94-087A-A748-AD59-ECCA265930F6}"/>
+    <hyperlink ref="A21" r:id="rId12" xr:uid="{C49F1946-962B-0849-89CF-B07B6FCF213D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>